<commit_message>
update sample files. rename of text fields
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d0512c548d3d688/tmp/111/1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\projects\electronic-death-certificate-format-tabular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{60992863-EA63-4EB8-9526-D71422F45C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{010CBDF2-4720-41F4-BFCC-C50B90113F8D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3C3DCD-3B67-45EA-8C95-ACFE542EA167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26496" yWindow="2532" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample" sheetId="1" r:id="rId1"/>
@@ -85,9 +85,6 @@
     <t>CauseOfDeathURIE</t>
   </si>
   <si>
-    <t>TextualCauseOfDeathE</t>
-  </si>
-  <si>
     <t>IntervalE</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>CauseOfDeathURIPart2</t>
   </si>
   <si>
-    <t>TextualCauseOfDeathPart2</t>
-  </si>
-  <si>
     <t>MaternalDeathWasPregnant</t>
   </si>
   <si>
@@ -212,6 +206,12 @@
   </si>
   <si>
     <t>CauseOfDeathTextD</t>
+  </si>
+  <si>
+    <t>CauseOfDeathTextPart2</t>
+  </si>
+  <si>
+    <t>CauseOfDeathTextE</t>
   </si>
 </sst>
 </file>
@@ -781,10 +781,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1086,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1127,7 +1123,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K1" t="s">
         <v>9</v>
@@ -1139,7 +1135,7 @@
         <v>11</v>
       </c>
       <c r="N1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O1" t="s">
         <v>12</v>
@@ -1151,7 +1147,7 @@
         <v>14</v>
       </c>
       <c r="R1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="S1" t="s">
         <v>15</v>
@@ -1163,7 +1159,7 @@
         <v>17</v>
       </c>
       <c r="V1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="W1" t="s">
         <v>18</v>
@@ -1175,31 +1171,31 @@
         <v>20</v>
       </c>
       <c r="Z1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA1" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE1" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>27</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.3">
@@ -1207,37 +1203,37 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
         <v>31</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>32</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M2" t="s">
         <v>33</v>
       </c>
-      <c r="L2" t="s">
+      <c r="P2" t="s">
         <v>34</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>35</v>
       </c>
-      <c r="P2" t="s">
+      <c r="T2" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="U2" t="s">
         <v>37</v>
-      </c>
-      <c r="T2" t="s">
-        <v>38</v>
-      </c>
-      <c r="U2" t="s">
-        <v>39</v>
       </c>
       <c r="AE2">
         <v>0</v>
@@ -1251,43 +1247,43 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
         <v>40</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>41</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
         <v>42</v>
       </c>
-      <c r="L3" t="s">
+      <c r="P3" t="s">
         <v>43</v>
       </c>
-      <c r="M3" t="s">
+      <c r="Q3" t="s">
         <v>44</v>
       </c>
-      <c r="P3" t="s">
+      <c r="T3" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="U3" t="s">
         <v>46</v>
       </c>
-      <c r="T3" t="s">
+      <c r="AB3" t="s">
         <v>47</v>
       </c>
-      <c r="U3" t="s">
+      <c r="AC3" t="s">
         <v>48</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>50</v>
       </c>
       <c r="AE3">
         <v>0</v>
@@ -1301,37 +1297,37 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" t="s">
         <v>51</v>
       </c>
-      <c r="H4" t="s">
+      <c r="L4" t="s">
         <v>52</v>
       </c>
-      <c r="I4" t="s">
+      <c r="M4" t="s">
         <v>53</v>
       </c>
-      <c r="L4" t="s">
+      <c r="P4" t="s">
         <v>54</v>
       </c>
-      <c r="M4" t="s">
+      <c r="Q4" t="s">
         <v>55</v>
       </c>
-      <c r="P4" t="s">
+      <c r="AB4" t="s">
         <v>56</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="AC4" t="s">
         <v>57</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>59</v>
       </c>
       <c r="AE4">
         <v>0</v>
@@ -1345,37 +1341,37 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" t="s">
         <v>51</v>
       </c>
-      <c r="H5" t="s">
+      <c r="L5" t="s">
         <v>52</v>
       </c>
-      <c r="I5" t="s">
+      <c r="M5" t="s">
         <v>53</v>
       </c>
-      <c r="L5" t="s">
+      <c r="P5" t="s">
         <v>54</v>
       </c>
-      <c r="M5" t="s">
+      <c r="Q5" t="s">
         <v>55</v>
       </c>
-      <c r="P5" t="s">
+      <c r="AB5" t="s">
         <v>56</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="AC5" t="s">
         <v>57</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>59</v>
       </c>
       <c r="AE5">
         <v>0</v>

</xml_diff>